<commit_message>
Updating excel file for conversion
</commit_message>
<xml_diff>
--- a/layoutGenerator/uploads/sample_files/example_excel_format.xlsx
+++ b/layoutGenerator/uploads/sample_files/example_excel_format.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grant Ward\Desktop\UofSC School\TheBackyardigans\layoutGenerator\uploads\sample_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F5A8FD-E57F-44E7-B5FB-BDBE2161EF6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BA0842-883D-44FD-B041-333F5A3DD061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1860" windowWidth="14400" windowHeight="7270" xr2:uid="{2E378315-C40A-433F-A886-1EBB4187EC79}"/>
+    <workbookView xWindow="2200" yWindow="2200" windowWidth="14400" windowHeight="7270" xr2:uid="{2E378315-C40A-433F-A886-1EBB4187EC79}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="11">
   <si>
     <t>Descriptor</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>Exterior</t>
+  </si>
+  <si>
+    <t>WINDOW</t>
   </si>
 </sst>
 </file>
@@ -417,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DECC682-D3AC-405B-A5DD-FF93AD75680E}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -493,10 +496,10 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>106.25</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>17.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -507,10 +510,10 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>106.25</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>15.75</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -521,10 +524,10 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>91.5</v>
+        <v>50</v>
       </c>
       <c r="D6">
-        <v>15.75</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -535,10 +538,10 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>91.5</v>
+        <v>50</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -549,10 +552,10 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -563,10 +566,10 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D9">
-        <v>100</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -574,13 +577,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C10">
-        <v>23.5</v>
+        <v>100</v>
       </c>
       <c r="D10">
-        <v>100</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -588,13 +591,55 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C11">
-        <v>23.5</v>
+        <v>100</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>100</v>
+      </c>
+      <c r="D12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>100</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>